<commit_message>
Updated Arbeitsprotokoll, new Controller
</commit_message>
<xml_diff>
--- a/Protokolle/ArbeitsProtokoll.xlsx
+++ b/Protokolle/ArbeitsProtokoll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/Documents/Schule/Diplomarbeit/Protokolle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\GitHub\maxxwell_webproject\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A09F18D-98DE-8743-BD10-752D9F670ED8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43612744-2A4A-4B63-A541-B8F474C6DD98}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15960" xr2:uid="{DA789707-4C3A-9940-BF61-CF9438299241}"/>
+    <workbookView xWindow="285" yWindow="465" windowWidth="28245" windowHeight="15960" xr2:uid="{DA789707-4C3A-9940-BF61-CF9438299241}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Arbeitspaket/Bezeichung</t>
   </si>
@@ -115,6 +115,54 @@
   </si>
   <si>
     <t>Daten-Kapitel</t>
+  </si>
+  <si>
+    <t>IMP…Implementierung</t>
+  </si>
+  <si>
+    <t>IMP</t>
+  </si>
+  <si>
+    <t>Datenbank-Erstellung</t>
+  </si>
+  <si>
+    <t>Datenbank-Verbindung/Deployment</t>
+  </si>
+  <si>
+    <t>View-Login</t>
+  </si>
+  <si>
+    <t>View-Register</t>
+  </si>
+  <si>
+    <t>Model-Datenbank-Operationen (laufend erweitert)</t>
+  </si>
+  <si>
+    <t>Model-DBConnector</t>
+  </si>
+  <si>
+    <t>Controller-Login</t>
+  </si>
+  <si>
+    <t>Controller-Register</t>
+  </si>
+  <si>
+    <t>Controller-Resets (4 zusammengefasst)</t>
+  </si>
+  <si>
+    <t>Controller-MailSender</t>
+  </si>
+  <si>
+    <t>Controller-Logout</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Server/Client-Beschreibung</t>
+  </si>
+  <si>
+    <t>Projektstrukturplan (PSP)</t>
   </si>
 </sst>
 </file>
@@ -467,24 +515,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A31150-A8ED-FE41-BD34-00B41D3ED644}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="11" max="11" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>9</v>
       </c>
@@ -498,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -524,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -542,17 +590,17 @@
       </c>
       <c r="H3">
         <f>SUM(E3:E343)</f>
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="I3">
         <f>SUM(F3:F343)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -572,7 +620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -592,7 +640,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -608,8 +656,11 @@
       <c r="G6" s="1">
         <v>43396</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -626,7 +677,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -643,7 +694,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -660,7 +711,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -677,7 +728,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -694,7 +745,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -711,7 +762,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -728,7 +779,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -745,7 +796,7 @@
         <v>43401</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -762,7 +813,7 @@
         <v>43404</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -779,7 +830,7 @@
         <v>43411</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -796,7 +847,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>27</v>
       </c>
@@ -807,13 +858,13 @@
         <v>25</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1">
         <v>43417</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>27</v>
       </c>
@@ -824,40 +875,245 @@
         <v>29</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1">
         <v>43434</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>43436</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>43436</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>43437</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>43456</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>43457</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>43457</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>43458</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>43458</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>43459</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>43460</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>43460</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1">
+        <v>43461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>43461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D46" t="s">
         <v>23</v>
       </c>
-      <c r="E25">
+      <c r="E46">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F46">
         <v>1</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G46" s="1">
         <v>43385</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="E47">
         <v>1</v>
       </c>
-      <c r="F26">
+      <c r="F47">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G47" s="1">
         <v>43426</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Controllers and Model
</commit_message>
<xml_diff>
--- a/Protokolle/ArbeitsProtokoll.xlsx
+++ b/Protokolle/ArbeitsProtokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\GitHub\maxxwell_webproject\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43612744-2A4A-4B63-A541-B8F474C6DD98}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3C12E-6388-4371-A2C1-C271265E355C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="465" windowWidth="28245" windowHeight="15960" xr2:uid="{DA789707-4C3A-9940-BF61-CF9438299241}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>Arbeitspaket/Bezeichung</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>Projektstrukturplan (PSP)</t>
+  </si>
+  <si>
+    <t>View-Benutzer</t>
+  </si>
+  <si>
+    <t>Controller-UserProfile</t>
+  </si>
+  <si>
+    <t>Model-Datenbank-Operationen</t>
+  </si>
+  <si>
+    <t>Controller-DeleteAccount</t>
+  </si>
+  <si>
+    <t>Controller-CreateAssignment</t>
   </si>
 </sst>
 </file>
@@ -517,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A31150-A8ED-FE41-BD34-00B41D3ED644}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -590,11 +605,11 @@
       </c>
       <c r="H3">
         <f>SUM(E3:E343)</f>
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="I3">
         <f>SUM(F3:F343)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -1084,6 +1099,133 @@
       </c>
       <c r="G33" s="1">
         <v>43461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>43462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1">
+        <v>43462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1">
+        <v>43463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>43463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>43463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="G39" s="1">
+        <v>43463</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="G40" s="1">
+        <v>43464</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>43464</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Controller + Database
</commit_message>
<xml_diff>
--- a/Protokolle/ArbeitsProtokoll.xlsx
+++ b/Protokolle/ArbeitsProtokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\GitHub\maxxwell_webproject\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3C12E-6388-4371-A2C1-C271265E355C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B581F9A-C755-49E7-9742-F4D421558307}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="465" windowWidth="28245" windowHeight="15960" xr2:uid="{DA789707-4C3A-9940-BF61-CF9438299241}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
       </c>
       <c r="H3">
         <f>SUM(E3:E343)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3">
         <f>SUM(F3:F343)</f>
@@ -1207,7 +1207,7 @@
         <v>47</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G41" s="1">
         <v>43464</v>

</xml_diff>

<commit_message>
Updated Controllers and Models
</commit_message>
<xml_diff>
--- a/Protokolle/ArbeitsProtokoll.xlsx
+++ b/Protokolle/ArbeitsProtokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\GitHub\maxxwell_webproject\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591012C3-F559-4541-BAAC-A096028EB9BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4BD229-9BFD-47BF-A561-0964630BC0F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="465" windowWidth="28245" windowHeight="15960" xr2:uid="{DA789707-4C3A-9940-BF61-CF9438299241}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>Arbeitspaket/Bezeichung</t>
   </si>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A31150-A8ED-FE41-BD34-00B41D3ED644}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="H3">
         <f>SUM(E3:E343)</f>
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I3">
         <f>SUM(F3:F343)</f>
@@ -1350,12 +1350,29 @@
       <c r="B50" t="s">
         <v>31</v>
       </c>
+      <c r="D50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1">
+        <v>43468</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="1"/>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>43468</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">

</xml_diff>